<commit_message>
Update File Type Currency Convertor
</commit_message>
<xml_diff>
--- a/Docs/PackageModule/Report.xlsx
+++ b/Docs/PackageModule/Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="TaskList" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="283">
   <si>
     <t>Project Name</t>
   </si>
@@ -856,6 +856,15 @@
   </si>
   <si>
     <t>Ajouter une politique d'annulation de package</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Add Available Languages</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1248,7 @@
     <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1316,15 +1325,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1370,7 +1382,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -1389,8 +1404,11 @@
       <c r="I8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -1410,12 +1428,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1519,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>